<commit_message>
adult tod norms through rnl
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/del_sum-adult-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/del_sum-adult-raw-ss-lookup-tabbed-age.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,202 +376,210 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>114</v>
+      <c r="B27">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +589,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -601,39 +609,39 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>55</v>
@@ -641,7 +649,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>56</v>
@@ -649,7 +657,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>57</v>
@@ -657,7 +665,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>58</v>
@@ -665,7 +673,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>59</v>
@@ -673,15 +681,15 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>62</v>
@@ -689,7 +697,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>63</v>
@@ -697,15 +705,15 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>66</v>
@@ -713,7 +721,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>68</v>
@@ -721,15 +729,15 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>71</v>
@@ -737,66 +745,74 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>110</v>
+      <c r="B27">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +822,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -826,135 +842,135 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>72</v>
@@ -962,7 +978,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>74</v>
@@ -970,15 +986,15 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>79</v>
@@ -986,42 +1002,50 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>110</v>
+      <c r="B27">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1031,7 +1055,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1051,47 +1075,47 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>58</v>
@@ -1099,7 +1123,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>59</v>
@@ -1107,7 +1131,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>60</v>
@@ -1115,7 +1139,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>62</v>
@@ -1123,7 +1147,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>63</v>
@@ -1131,7 +1155,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>64</v>
@@ -1139,7 +1163,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>66</v>
@@ -1147,106 +1171,114 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>111</v>
+      <c r="B27">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1256,7 +1288,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1276,202 +1308,210 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>115</v>
+      <c r="B27">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1521,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1501,201 +1541,209 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>113</v>
       </c>
     </row>

</xml_diff>